<commit_message>
Fix accumulatoin of PlantWaterOnNDelta classes
</commit_message>
<xml_diff>
--- a/Prototypes/STRUM/TreeRadIntScheme.xlsx
+++ b/Prototypes/STRUM/TreeRadIntScheme.xlsx
@@ -8,31 +8,49 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\ApsimX\Prototypes\STRUM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F457F0-72BE-4051-B4ED-778009C09444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14CC83C7-BFCB-4344-9019-AA1203B26D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-5925" windowWidth="16440" windowHeight="28320" xr2:uid="{229C4D6A-5FB6-4819-BCE2-E59B5C06DA37}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Crop" sheetId="2" r:id="rId1"/>
+    <sheet name="Tree" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="CBHt">Sheet1!#REF!</definedName>
-    <definedName name="CDt">Sheet1!#REF!</definedName>
-    <definedName name="CWt">Sheet1!#REF!</definedName>
-    <definedName name="Fa">Sheet1!#REF!</definedName>
-    <definedName name="Fabla">Sheet1!#REF!</definedName>
-    <definedName name="Ft">Sheet1!#REF!</definedName>
-    <definedName name="Ftbla">Sheet1!#REF!</definedName>
-    <definedName name="Ht">Sheet1!#REF!</definedName>
-    <definedName name="Ka">Sheet1!#REF!</definedName>
-    <definedName name="Kt">Sheet1!#REF!</definedName>
-    <definedName name="LAIa">Sheet1!#REF!</definedName>
-    <definedName name="LAIt">Sheet1!#REF!</definedName>
-    <definedName name="LAIthomo">Sheet1!#REF!</definedName>
-    <definedName name="Wa">Sheet1!#REF!</definedName>
-    <definedName name="WaOL">Sheet1!#REF!</definedName>
-    <definedName name="WaOp">Sheet1!#REF!</definedName>
-    <definedName name="Wt">Sheet1!#REF!</definedName>
+    <definedName name="CBHt" localSheetId="0">Crop!#REF!</definedName>
+    <definedName name="CBHt">Tree!#REF!</definedName>
+    <definedName name="CDt" localSheetId="0">Crop!#REF!</definedName>
+    <definedName name="CDt">Tree!#REF!</definedName>
+    <definedName name="CWt" localSheetId="0">Crop!#REF!</definedName>
+    <definedName name="CWt">Tree!#REF!</definedName>
+    <definedName name="Fa" localSheetId="0">Crop!#REF!</definedName>
+    <definedName name="Fa">Tree!#REF!</definedName>
+    <definedName name="Fabla" localSheetId="0">Crop!#REF!</definedName>
+    <definedName name="Fabla">Tree!#REF!</definedName>
+    <definedName name="Ft" localSheetId="0">Crop!#REF!</definedName>
+    <definedName name="Ft">Tree!#REF!</definedName>
+    <definedName name="Ftbla" localSheetId="0">Crop!#REF!</definedName>
+    <definedName name="Ftbla">Tree!#REF!</definedName>
+    <definedName name="Ht" localSheetId="0">Crop!#REF!</definedName>
+    <definedName name="Ht">Tree!#REF!</definedName>
+    <definedName name="Ka" localSheetId="0">Crop!#REF!</definedName>
+    <definedName name="Ka">Tree!#REF!</definedName>
+    <definedName name="Kt" localSheetId="0">Crop!#REF!</definedName>
+    <definedName name="Kt">Tree!#REF!</definedName>
+    <definedName name="LAIa" localSheetId="0">Crop!#REF!</definedName>
+    <definedName name="LAIa">Tree!#REF!</definedName>
+    <definedName name="LAIt" localSheetId="0">Crop!#REF!</definedName>
+    <definedName name="LAIt">Tree!#REF!</definedName>
+    <definedName name="LAIthomo" localSheetId="0">Crop!#REF!</definedName>
+    <definedName name="LAIthomo">Tree!#REF!</definedName>
+    <definedName name="Wa" localSheetId="0">Crop!#REF!</definedName>
+    <definedName name="Wa">Tree!#REF!</definedName>
+    <definedName name="WaOL" localSheetId="0">Crop!#REF!</definedName>
+    <definedName name="WaOL">Tree!#REF!</definedName>
+    <definedName name="WaOp" localSheetId="0">Crop!#REF!</definedName>
+    <definedName name="WaOp">Tree!#REF!</definedName>
+    <definedName name="Wt" localSheetId="0">Crop!#REF!</definedName>
+    <definedName name="Wt">Tree!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -55,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
     <t>CanopyWidth</t>
   </si>
@@ -176,7 +194,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$7</c:f>
+              <c:f>Crop!$C$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -187,7 +205,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$7:$A$12</c:f>
+              <c:f>Crop!$A$7:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -198,40 +216,40 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9.9990000000000006</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$7:$D$12</c:f>
+              <c:f>Crop!$D$7:$D$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.98995000380031117</c:v>
+                  <c:v>0.97980006161982436</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.98895061537887097</c:v>
+                  <c:v>0.97531245118712795</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.98019998000399899</c:v>
+                  <c:v>0.96722206798690891</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>0.95124921972503929</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0.90498756211208897</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4.9998750062563114E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -242,7 +260,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000008-2713-4284-A645-C16434EFA236}"/>
+              <c16:uniqueId val="{00000000-EB51-4E4B-A728-0E8A51EE1070}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -251,11 +269,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$13</c:f>
+              <c:f>Crop!$C$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -271,7 +289,7 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$13:$A$18</c:f>
+              <c:f>Crop!$A$13:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -282,40 +300,40 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9.9990000000000006</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$13:$D$18</c:f>
+              <c:f>Crop!$D$13:$D$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.90407847245298978</c:v>
+                  <c:v>0.9600163130807533</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.89504279312637969</c:v>
+                  <c:v>0.95124921972503929</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.81980390271855685</c:v>
+                  <c:v>0.93555309189152702</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.41421356237309515</c:v>
+                  <c:v>0.90498756211208897</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.9999987505905353E-4</c:v>
+                  <c:v>0.81980390271855708</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -326,7 +344,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000009-2713-4284-A645-C16434EFA236}"/>
+              <c16:uniqueId val="{00000001-EB51-4E4B-A728-0E8A51EE1070}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -335,18 +353,18 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$19</c:f>
+              <c:f>Crop!$C$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$19:$A$24</c:f>
+              <c:f>Crop!$A$19:$A$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -357,40 +375,40 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9.9990000000000006</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$19:$D$24</c:f>
+              <c:f>Crop!$D$19:$D$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.81818181818181812</c:v>
+                  <c:v>0.90315186579793894</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.80217160636587637</c:v>
+                  <c:v>0.88278221853731864</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.67703296142690073</c:v>
+                  <c:v>0.84712708838303652</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.23606797749978981</c:v>
+                  <c:v>0.78077640640441515</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.499999842699161E-4</c:v>
+                  <c:v>0.6180339887498949</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -401,7 +419,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-2713-4284-A645-C16434EFA236}"/>
+              <c16:uniqueId val="{00000002-EB51-4E4B-A728-0E8A51EE1070}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -410,11 +428,11 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$25</c:f>
+              <c:f>Crop!$C$25</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -445,7 +463,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$25:$A$30</c:f>
+              <c:f>Crop!$A$25:$A$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -456,23 +474,596 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9.9990000000000006</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$25:$D$30</c:f>
+              <c:f>Crop!$D$25:$D$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.81653059184081533</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.78077640640441515</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.72075922005612647</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.6180339887498949</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.41421356237309515</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-EB51-4E4B-A728-0E8A51EE1070}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1696214784"/>
+        <c:axId val="1925498384"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1696214784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Canopy</a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t> Width</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1925498384"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1925498384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1696214784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="l"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tree!$C$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tree!$A$7:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.9990000000000006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tree!$D$7:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.98995000380031117</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.98895061537887097</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.98019998000399899</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.90498756211208897</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.9998750062563114E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-2713-4284-A645-C16434EFA236}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tree!$C$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tree!$A$13:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.9990000000000006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tree!$D$13:$D$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.90407847245298978</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.89504279312637969</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.81980390271855685</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.41421356237309515</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.9999987505905353E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-2713-4284-A645-C16434EFA236}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tree!$C$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tree!$A$19:$A$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.9990000000000006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tree!$D$19:$D$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.81818181818181812</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.80217160636587637</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.67703296142690073</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.23606797749978981</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.499999842699161E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-2713-4284-A645-C16434EFA236}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tree!$C$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tree!$A$25:$A$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.9990000000000006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tree!$D$25:$D$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -695,6 +1286,49 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{527A5A7A-31F3-41A6-A5D2-9B6F9E6C4CFF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1051,11 +1685,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53FD53D9-BFF3-48EC-B4F4-5ACE7414F6FC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F338973-175B-459B-A4E9-DBF33990CE94}">
   <dimension ref="A6:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="C25" sqref="C25:C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1084,6 +1718,425 @@
         <v>0.1</v>
       </c>
       <c r="B7">
+        <f>MAX(0,5-A7)</f>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="C7">
+        <v>0.1</v>
+      </c>
+      <c r="D7">
+        <f>(SQRT(POWER(C7, 2) + POWER(B7, 2)) - C7) / B7</f>
+        <v>0.97980006161982436</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <f t="shared" ref="B8:B30" si="0">MAX(0,5-A8)</f>
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>0.1</v>
+      </c>
+      <c r="D8">
+        <f t="shared" ref="D8:D30" si="1">(SQRT(POWER(C8, 2) + POWER(B8, 2)) - C8) / B8</f>
+        <v>0.97531245118712795</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>0.1</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>0.96722206798690891</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>0.1</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>0.95124921972503929</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>0.1</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>0.90498756211208897</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0.1</v>
+      </c>
+      <c r="D12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0.1</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="C13">
+        <v>0.2</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>0.9600163130807533</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>0.2</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>0.95124921972503929</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>0.2</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>0.93555309189152702</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>0.2</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>0.90498756211208897</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>0.2</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>0.81980390271855708</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0.2</v>
+      </c>
+      <c r="D18" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>0.1</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="C19">
+        <v>0.5</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>0.90315186579793894</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C20">
+        <v>0.5</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>0.88278221853731864</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C21">
+        <v>0.5</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="1"/>
+        <v>0.84712708838303652</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>0.5</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="1"/>
+        <v>0.78077640640441515</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>4</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>0.5</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="1"/>
+        <v>0.6180339887498949</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0.5</v>
+      </c>
+      <c r="D24" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>0.1</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="1"/>
+        <v>0.81653059184081533</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="1"/>
+        <v>0.78077640640441515</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>2</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="1"/>
+        <v>0.72075922005612647</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>3</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="1"/>
+        <v>0.6180339887498949</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>4</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="1"/>
+        <v>0.41421356237309515</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>5</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53FD53D9-BFF3-48EC-B4F4-5ACE7414F6FC}">
+  <dimension ref="A6:D30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0.1</v>
+      </c>
+      <c r="B7">
         <f>MAX(0,10-A7)</f>
         <v>9.9</v>
       </c>

</xml_diff>